<commit_message>
Send Description with Json
</commit_message>
<xml_diff>
--- a/Plan/Mumbai.xlsx
+++ b/Plan/Mumbai.xlsx
@@ -279,7 +279,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -300,7 +299,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -308,13 +306,11 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,8 +455,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1200,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Final data for Mi
</commit_message>
<xml_diff>
--- a/Plan/Mumbai.xlsx
+++ b/Plan/Mumbai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="930" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="170">
   <si>
     <t>id</t>
   </si>
@@ -62,33 +62,42 @@
     <t>Timings</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
+    <t>P.S</t>
+  </si>
+  <si>
+    <t>P.P.S</t>
+  </si>
+  <si>
     <t>Marine drive</t>
   </si>
   <si>
+    <t>5 AM - 2 AM</t>
+  </si>
+  <si>
+    <t>Also known as the Queen's necklace for its beautiful 'C' shape that brushes sides with the Arabian sea, is the Marine drive, separating the sea from the city, which in every other metaphorical sense of the word, are one.</t>
+  </si>
+  <si>
+    <t>P.S : Try Girgaum Chowpatty along with the visit</t>
+  </si>
+  <si>
+    <t>P.P.S : There is a aquarium named Taraporewala just next to it</t>
+  </si>
+  <si>
+    <t>Gateway of India</t>
+  </si>
+  <si>
     <t>5 AM - 11:59 PM</t>
   </si>
   <si>
-    <t>Try Girgaum Chowpatty along with the visit</t>
-  </si>
-  <si>
-    <t>Also known as the Queen's necklace for its beautiful 'C' shape that brushes sides with the Arabian sea, is the Marine drive, separating the sea from the city, which in every other metaphorical sense of the word, are one.</t>
-  </si>
-  <si>
-    <t>Gateway of India</t>
-  </si>
-  <si>
-    <t>Try ferry/yacht ride if you are interested in that. And if non-veg, try Bademiya</t>
-  </si>
-  <si>
     <t>Facing the Arabian sea on one side and the city landmarked by the most recognized hotels of India, The Taj on the other, is the one place in Mumbai, its visitors just cannot miss.</t>
   </si>
   <si>
+    <t>P.S : If you are hardcore non vegiterian try Bade Miya or baghdadi</t>
+  </si>
+  <si>
     <t>18.982831</t>
   </si>
   <si>
@@ -131,12 +140,15 @@
     <t>10 AM - 8 PM</t>
   </si>
   <si>
-    <t>Check its site for offers</t>
-  </si>
-  <si>
     <t>If you are looking forward for amusement, essel world and water kingdom is the place for you.</t>
   </si>
   <si>
+    <t>P.S : Don't follow google maps to reach there, you can find direct ferry from Marve(Malad) and Gorai (Borivali)</t>
+  </si>
+  <si>
+    <t>P.P.S : Check www.esselworld.in for offers</t>
+  </si>
+  <si>
     <t>19.117639</t>
   </si>
   <si>
@@ -146,12 +158,12 @@
     <t>Juhu Beach</t>
   </si>
   <si>
-    <t>Try Juhu chowpaty</t>
-  </si>
-  <si>
     <t>The most popular beach in Mumbai, Juhu beach is located close to Andheri and was once quite a beautiful beach. However, with so many tourists coming in here, the place has become dirty and water is also not clean because of affluents from nearby factories and industries.</t>
   </si>
   <si>
+    <t>P.S : Don't forget to try Bhel, Pav Bhaji and gola</t>
+  </si>
+  <si>
     <t>18.9176046</t>
   </si>
   <si>
@@ -164,12 +176,12 @@
     <t>9 AM -10 PM</t>
   </si>
   <si>
-    <t>Along this street is an Afgan church and Sasson dock.</t>
-  </si>
-  <si>
     <t>Colaba causeway is a hub of shopping market for apparels, gadgets, accessories, footwear, etc.</t>
   </si>
   <si>
+    <t>P.S : Along this street is an Afgan church and Sasson dock.</t>
+  </si>
+  <si>
     <t>19.024121</t>
   </si>
   <si>
@@ -182,12 +194,15 @@
     <t>All day</t>
   </si>
   <si>
-    <t>You can sit there for while at worli sea face</t>
-  </si>
-  <si>
     <t>A cable stayed bridge linking the western suburbs of Mumbai to its southern part is a wide freeway of eight lanes and a recent addition to the prominent landmarks of the city.</t>
   </si>
   <si>
+    <t>P.S : Only four wheelers are allowed on bridge, ou  can always go by a cab</t>
+  </si>
+  <si>
+    <t>P.P.S : Worli sea face is nace place to spend some quality time</t>
+  </si>
+  <si>
     <t>18.9632529</t>
   </si>
   <si>
@@ -203,6 +218,9 @@
     <t>A drive from Mumbai or a ferry ride away from Gateway of India are famous Elephants caves, a favorite on the lists of a history enthusiasts.</t>
   </si>
   <si>
+    <t>P.S : You have to board a ferry from gateway of India</t>
+  </si>
+  <si>
     <t>19.0473121</t>
   </si>
   <si>
@@ -233,6 +251,12 @@
     <t>The gallery is a true ode to Indian glory in the form of art. </t>
   </si>
   <si>
+    <t>P.S : Nice place for art lovers</t>
+  </si>
+  <si>
+    <t>P.P.S : You can find artist outside who will make your sketch for 100-150 bucks</t>
+  </si>
+  <si>
     <t>19.2107217</t>
   </si>
   <si>
@@ -242,25 +266,28 @@
     <t>Sanjay Gandhi National park</t>
   </si>
   <si>
-    <t>7:30 AM - 6:30 PM</t>
-  </si>
-  <si>
-    <t>You should have a look at Kanheri caves alongwith it</t>
+    <t>9 AM – 5.30 PM</t>
   </si>
   <si>
     <t>This is a wildlife sanctuary and a habitat to abundance of flora and fauna, in the midst of a busy Mumbai.</t>
   </si>
   <si>
-    <t>19.1301305</t>
-  </si>
-  <si>
-    <t>72.8735171</t>
-  </si>
-  <si>
-    <t>Mahakali caves</t>
-  </si>
-  <si>
-    <t>Located on Udyagiri hills, these cave are carved out of hard rock. There are 19 caves in all and served as a Buddhist Monastery.</t>
+    <t>P.S : Kanheri caves is a good place a spend some quality time.</t>
+  </si>
+  <si>
+    <t>P.P.S : Get a ride of wild life safari bus, and you maybe get a chance to see tigers</t>
+  </si>
+  <si>
+    <t>Band Stand</t>
+  </si>
+  <si>
+    <t>BandStand in Bandra is a great place to enjoy the sea breeze. You can go at any time of the day and still feel good. The sound of the waves splashing on the rocks creates a soothing music to the ears</t>
+  </si>
+  <si>
+    <t>P.S : Foodies try Candies near Pali hill. It's romantic place</t>
+  </si>
+  <si>
+    <t>P.P.S : Lookout for bunglows of film stars like Shahrukh, Amitabh</t>
   </si>
   <si>
     <t>19.2280556</t>
@@ -278,6 +305,9 @@
     <t>The Burmese architectural style Pagoda is a monument for peace and harmony.</t>
   </si>
   <si>
+    <t>P.S : Get a ferry from Gorai (Borivali) or Marve (Malad)</t>
+  </si>
+  <si>
     <t>19.055491</t>
   </si>
   <si>
@@ -293,108 +323,117 @@
     <t>Acknowledged for its high fashionable taste, Mumbai provides many opportunities to shop around.</t>
   </si>
   <si>
-    <t>19.161095</t>
-  </si>
-  <si>
-    <t>72.887362</t>
-  </si>
-  <si>
-    <t>Film City</t>
+    <t>Chhatrapati Shivaji Museum</t>
+  </si>
+  <si>
+    <t>11 AM – 5.30 PM</t>
+  </si>
+  <si>
+    <t>The Museum building, a Grade I Heritage building, is a fine example of the Indo-Saracenic style of architecture and houses a world-class collection of over 60,000 art objects.</t>
+  </si>
+  <si>
+    <t>18.9567</t>
+  </si>
+  <si>
+    <t>72.804917</t>
+  </si>
+  <si>
+    <t>Hanging Gardens</t>
+  </si>
+  <si>
+    <t>5 AM - 9 PM</t>
+  </si>
+  <si>
+    <t>Marked by bushes trimmed into shapes of various animals and proximity to the Arabian Sea are the Hanging Gardens</t>
+  </si>
+  <si>
+    <t>P.S : One can chill out too in Kamla Nehru Park, situated opposite to it</t>
+  </si>
+  <si>
+    <t>18.9385</t>
+  </si>
+  <si>
+    <t>72.830061</t>
+  </si>
+  <si>
+    <t>Fashion Street</t>
+  </si>
+  <si>
+    <t>11 AM - 8 PM</t>
+  </si>
+  <si>
+    <t>This street provides all sorts of shopping experiences at real cheap rates. Enjoy your shopping for hats, footwear, books, etc here.</t>
+  </si>
+  <si>
+    <t> P.S : Negotiate properly ;). You ca  buy at 5 times less than quated price</t>
+  </si>
+  <si>
+    <t>19.146726</t>
+  </si>
+  <si>
+    <t>72.829554</t>
+  </si>
+  <si>
+    <t>Lokhandwala Market</t>
+  </si>
+  <si>
+    <t>Lokhandwala is another place to shop happily and heartily.</t>
+  </si>
+  <si>
+    <t>P.S : Do not miss the lip-smacking food around these shopping streets.</t>
+  </si>
+  <si>
+    <t>Bar stock exchange</t>
+  </si>
+  <si>
+    <t>6 PM –  1 AM</t>
+  </si>
+  <si>
+    <t>A unique experience, as name says it all it works similar to stock excange, but you buy booze here</t>
+  </si>
+  <si>
+    <t>P.S : Stag entry not allowed on weekends</t>
+  </si>
+  <si>
+    <t>P.P.S : They might ask you to provide proof of being older than 21</t>
+  </si>
+  <si>
+    <t>Blue frog</t>
+  </si>
+  <si>
+    <t>This luxurious club features regular parties with live acts, a global menu and modern design.</t>
+  </si>
+  <si>
+    <t>P.S : Live performance on every Thursday</t>
+  </si>
+  <si>
+    <t>Nehru Planetarium</t>
+  </si>
+  <si>
+    <t>10:30 AM - 5 PM</t>
+  </si>
+  <si>
+    <t>The planetarium is one of the premiere astronomical institutes in India. All the activities held in the planetarium are directed towards encouraging young minds to be fascinated with and try to find out more about our universe.</t>
+  </si>
+  <si>
+    <t>P.S : You can enjoy a dome show at 3 PM</t>
+  </si>
+  <si>
+    <t>Nehru Science Center</t>
+  </si>
+  <si>
+    <t>10 AM - 6 PM</t>
+  </si>
+  <si>
+    <t>Science museum featuring interactive exhibits for kids &amp; adults, plus seminars, events &amp; lMAX films.</t>
+  </si>
+  <si>
+    <t>Mount Mary Church</t>
   </si>
   <si>
     <t>10 AM - 5 PM</t>
   </si>
   <si>
-    <t>One can take tours through the film city to experience the fascinating world of movies</t>
-  </si>
-  <si>
-    <t>18.9567</t>
-  </si>
-  <si>
-    <t>72.804917</t>
-  </si>
-  <si>
-    <t>Hanging Gardens</t>
-  </si>
-  <si>
-    <t>5 AM - 9 PM</t>
-  </si>
-  <si>
-    <t>One can chill out too in Kamla Nehru Park, situated opposite to it</t>
-  </si>
-  <si>
-    <t>Marked by bushes trimmed into shapes of various animals and proximity to the Arabian Sea are the Hanging Gardens</t>
-  </si>
-  <si>
-    <t>18.9385</t>
-  </si>
-  <si>
-    <t>72.830061</t>
-  </si>
-  <si>
-    <t>Fashion Street</t>
-  </si>
-  <si>
-    <t>11 AM - 8 PM</t>
-  </si>
-  <si>
-    <t>Negotiate properly ;)</t>
-  </si>
-  <si>
-    <t>This street provides all sorts of shopping experiences at real cheap rates. Enjoy your shopping for hats, footwear, books, etc here.</t>
-  </si>
-  <si>
-    <t>19.146726</t>
-  </si>
-  <si>
-    <t>72.829554</t>
-  </si>
-  <si>
-    <t>Lokhandwala Market</t>
-  </si>
-  <si>
-    <t>Do not miss the lip-smacking food around these shopping streets.</t>
-  </si>
-  <si>
-    <t>Lokhandwala is another place to shop happily and heartily.</t>
-  </si>
-  <si>
-    <t>Tarapurwala Aquarium</t>
-  </si>
-  <si>
-    <t>India's oldest aquarium and one of the city's main attractions. it hosts marine and freshwater fishes.</t>
-  </si>
-  <si>
-    <t>Dhobi Ghat</t>
-  </si>
-  <si>
-    <t>7 AM - 4 PM</t>
-  </si>
-  <si>
-    <t>Dhobi ghat is somewhat of a distinguishing mark for Mumbai. The washers, known as Dhobis in the local tongue, who work in an open place wash the clothes of the citizens for a small fee. There are rows of open air washing and little cubicles are made with marble stone where the dhobis can wash their clothes.</t>
-  </si>
-  <si>
-    <t>Nehru Planetarium</t>
-  </si>
-  <si>
-    <t>10:30 AM - 5 PM</t>
-  </si>
-  <si>
-    <t>The planetarium is one of the premiere astronomical institutes in India. All the activities held in the planetarium are directed towards encouraging young minds to be fascinated with and try to find out more about our universe.</t>
-  </si>
-  <si>
-    <t>Nehru Science Center</t>
-  </si>
-  <si>
-    <t>10 AM - 6 PM</t>
-  </si>
-  <si>
-    <t>Science museum featuring interactive exhibits for kids &amp; adults, plus seminars, events &amp; lMAX films.</t>
-  </si>
-  <si>
-    <t>Mount Mary Church</t>
-  </si>
-  <si>
     <t>It has a beautiful statue of the Virgin Mary made of pure basalt. Regular prayer takes place.</t>
   </si>
   <si>
@@ -407,6 +446,9 @@
     <t>One of the most happening and most frequented malls of Mumbai.</t>
   </si>
   <si>
+    <t>P.S : Standup comedy fan? Lookout for Canvas laugh factory</t>
+  </si>
+  <si>
     <t>Aksa Beach</t>
   </si>
   <si>
@@ -440,12 +482,15 @@
     <t>11 AM - 11:59 PM</t>
   </si>
   <si>
-    <t>Check out pricing of different activities at their site</t>
-  </si>
-  <si>
     <t>A complete package of fun activities : skykarting, bowling, virtual games and a lot more. You can enjoy some beers ther too :D</t>
   </si>
   <si>
+    <t>P.S : Check out pricing of different activities at smaaash.in</t>
+  </si>
+  <si>
+    <t>P.P.S : Heaven for game lovers</t>
+  </si>
+  <si>
     <t>Hard Rock Cafe, Worli</t>
   </si>
   <si>
@@ -461,22 +506,25 @@
     <t>12:01 AM - 11:59 PM</t>
   </si>
   <si>
-    <t>If you reach there before 8, you can enjoy their Rs 77 menu</t>
-  </si>
-  <si>
     <t>Perfect Music, perfect ambience and cheap alcohol :D</t>
   </si>
   <si>
+    <t>P.S : If you reach there before 8 lookout for Rs 77 menu</t>
+  </si>
+  <si>
     <t>Colaba Social</t>
   </si>
   <si>
     <t>9 AM - 1 AM</t>
   </si>
   <si>
-    <t>On weekends, stag entry is not allowed; better book your tables befor time</t>
-  </si>
-  <si>
-    <t>Long Island Ice Tea is 'must' try</t>
+    <t>Perfect for socializing with your besties. Especially for a day out with girls. Crazy menu! And presentation is appealing. To the extent it really hurts to eat the food. </t>
+  </si>
+  <si>
+    <t>P.S : On weekends, stag entry is not allowed. Try Very lond island icetea</t>
+  </si>
+  <si>
+    <t>P.P.S : Officially you need to be older than 21 years or you need to have good convicing skills</t>
   </si>
 </sst>
 </file>
@@ -604,7 +652,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -629,7 +677,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -719,10 +775,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -730,7 +786,9 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.995951417004"/>
     <col collapsed="false" hidden="false" max="13" min="3" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.004048582996"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="38.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,6 +843,9 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -827,16 +888,19 @@
         <v>120</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,22 +938,22 @@
         <v>720</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>870</v>
+        <v>900</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,10 +961,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>25</v>
@@ -933,25 +997,25 @@
         <v>90</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>35</v>
@@ -984,25 +1048,25 @@
         <v>120</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -1032,19 +1096,22 @@
         <v>360</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>660</v>
+        <v>420</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,10 +1119,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>40</v>
@@ -1088,16 +1155,16 @@
         <v>120</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,10 +1172,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>15</v>
@@ -1141,16 +1208,16 @@
         <v>180</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,10 +1225,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>35</v>
@@ -1194,16 +1261,19 @@
         <v>60</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,16 +1281,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>806</v>
+        <v>700</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>80</v>
@@ -1238,23 +1308,25 @@
         <v>0</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>240</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="P10" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="Q10" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,10 +1334,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>15</v>
@@ -1295,34 +1367,34 @@
         <v>645</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>413</v>
+        <v>90</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>1</v>
@@ -1343,20 +1415,25 @@
         <v>360</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>720</v>
+        <v>810</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="P12" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="Q12" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,22 +1441,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1</v>
@@ -1391,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="L13" s="0" t="n">
         <v>510</v>
@@ -1400,33 +1477,36 @@
         <v>240</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>1</v>
+      <c r="B14" s="0" t="n">
+        <v>19.0505835</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>72.8192191</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>45</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>1</v>
@@ -1435,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>1</v>
@@ -1443,24 +1523,29 @@
       <c r="J14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K14" s="1" t="n">
-        <v>0</v>
+      <c r="K14" s="0" t="n">
+        <v>720</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>720</v>
+        <v>900</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>80</v>
+        <v>120</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P14" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="Q14" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,10 +1553,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>10</v>
@@ -1504,14 +1589,16 @@
         <v>240</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="P15" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="Q15" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,10 +1606,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>1</v>
@@ -1546,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>840</v>
@@ -1555,34 +1642,36 @@
         <v>120</v>
       </c>
       <c r="N16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="O16" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>1</v>
+      <c r="B17" s="0" t="n">
+        <v>18.9272722</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>72.8318454</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>40</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>1</v>
@@ -1596,24 +1685,23 @@
       <c r="J17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K17" s="1" t="n">
+      <c r="K17" s="0" t="n">
         <v>360</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>480</v>
+        <v>660</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>180</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>94</v>
+        <v>120</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,16 +1709,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1</v>
@@ -1648,25 +1736,25 @@
         <v>0</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>195</v>
+        <v>780</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>75</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,10 +1762,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
@@ -1695,13 +1783,13 @@
         <v>1</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="L19" s="0" t="n">
         <v>840</v>
@@ -1710,16 +1798,16 @@
         <v>90</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,10 +1815,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
@@ -1754,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>840</v>
@@ -1763,30 +1851,30 @@
         <v>120</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="P20" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="n">
-        <v>18.9492902</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>72.8180241</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>1</v>
+      <c r="B21" s="0" t="n">
+        <v>19.1393792</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>72.8434279</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -1798,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>1</v>
@@ -1806,37 +1894,43 @@
       <c r="J21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K21" s="1" t="n">
-        <v>0</v>
+      <c r="K21" s="0" t="n">
+        <v>810</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>195</v>
+        <v>960</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>114</v>
+        <v>180</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="n">
-        <v>18.9825286</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>72.8232678</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>1</v>
+      <c r="B22" s="0" t="n">
+        <v>19.0007441</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>72.8273683</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
@@ -1848,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>1</v>
@@ -1856,23 +1950,26 @@
       <c r="J22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K22" s="1" t="n">
-        <v>300</v>
+      <c r="K22" s="0" t="n">
+        <v>810</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>675</v>
+        <v>960</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>116</v>
+        <v>180</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>127</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,16 +2010,19 @@
         <v>600</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>121</v>
+        <v>131</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1966,13 +2066,13 @@
         <v>180</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>124</v>
+        <v>135</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,13 +2116,13 @@
         <v>45</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,13 +2166,16 @@
         <v>120</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>129</v>
+        <v>141</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="L27" s="0" t="n">
         <v>360</v>
@@ -2116,13 +2219,13 @@
         <v>120</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q27" s="8" t="s">
-        <v>131</v>
+        <v>24</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2245,7 @@
         <v>130</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>1</v>
@@ -2163,16 +2266,16 @@
         <v>360</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>133</v>
+        <v>108</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,13 +2319,13 @@
         <v>120</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q29" s="8" t="s">
-        <v>135</v>
+        <v>108</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>570</v>
+        <v>660</v>
       </c>
       <c r="L30" s="0" t="n">
         <v>840</v>
@@ -2266,13 +2369,13 @@
         <v>180</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q30" s="0" t="s">
-        <v>138</v>
+        <v>151</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,16 +2419,19 @@
         <v>210</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="P31" s="0" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="Q31" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,7 +2445,7 @@
         <v>72.827239</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
@@ -2369,13 +2475,13 @@
         <v>180</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q32" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
+      </c>
+      <c r="P32" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2419,19 +2525,19 @@
         <v>150</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="P33" s="0" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="Q33" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
@@ -2442,7 +2548,7 @@
         <v>72.8301393</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
@@ -2472,19 +2578,27 @@
         <v>150</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="P34" s="0" t="s">
-        <v>152</v>
+        <v>166</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="Q34" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
+        <v>168</v>
+      </c>
+      <c r="R34" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R6" r:id="rId1" display="www.esselworld.in"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Make Userdb and MumbaiDb
</commit_message>
<xml_diff>
--- a/Plan/Mumbai.xlsx
+++ b/Plan/Mumbai.xlsx
@@ -26,10 +26,10 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Default Happiness</t>
-  </si>
-  <si>
-    <t>Sigh Seeing</t>
+    <t>DefaultHappiness</t>
+  </si>
+  <si>
+    <t>SightSeeing</t>
   </si>
   <si>
     <t>Religious</t>
@@ -38,7 +38,7 @@
     <t>Amusement</t>
   </si>
   <si>
-    <t>Night Life</t>
+    <t>NightLife</t>
   </si>
   <si>
     <t>Shopping</t>
@@ -47,13 +47,13 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Open Time</t>
-  </si>
-  <si>
-    <t>Due time</t>
-  </si>
-  <si>
-    <t>Service time</t>
+    <t>OpenTime</t>
+  </si>
+  <si>
+    <t>Duetime</t>
+  </si>
+  <si>
+    <t>Servicetime</t>
   </si>
   <si>
     <t>Names</t>
@@ -65,10 +65,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>P.S</t>
-  </si>
-  <si>
-    <t>P.P.S</t>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>PPS</t>
   </si>
   <si>
     <t>Marine drive</t>
@@ -365,7 +365,7 @@
     <t>This street provides all sorts of shopping experiences at real cheap rates. Enjoy your shopping for hats, footwear, books, etc here.</t>
   </si>
   <si>
-    <t> P.S : Negotiate properly ;). You ca  buy at 5 times less than quated price</t>
+    <t>P.S : Negotiate properly ;). You ca  buy at 5 times less than quated price</t>
   </si>
   <si>
     <t>19.146726</t>
@@ -777,8 +777,8 @@
   </sheetPr>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2597,7 +2597,7 @@
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R6" r:id="rId1" display="www.esselworld.in"/>
+    <hyperlink ref="R6" r:id="rId1" display="P.P.S : Check www.esselworld.in for offers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Removed distance consideration for DDP
</commit_message>
<xml_diff>
--- a/Plan/Mumbai.xlsx
+++ b/Plan/Mumbai.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhoumik Shah\Desktop\TripieServer\Plan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="930" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="930"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -530,32 +534,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="HH:MM\ AM/PM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -569,7 +557,7 @@
       <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -596,7 +584,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Latoregular"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -608,7 +595,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -616,89 +603,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -757,33 +686,307 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.995951417004"/>
-    <col collapsed="false" hidden="false" max="13" min="3" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.004048582996"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="38.919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.5748987854251"/>
+    <col min="1" max="2" width="11"/>
+    <col min="3" max="13" width="8.5546875"/>
+    <col min="14" max="14" width="19"/>
+    <col min="15" max="16" width="8.5546875"/>
+    <col min="17" max="17" width="38.88671875"/>
+    <col min="18" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,16 +1020,16 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -835,48 +1038,48 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="n">
+    <row r="2" spans="1:18">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
         <v>18.943804</v>
       </c>
-      <c r="C2" s="4" t="n">
-        <v>72.822694</v>
-      </c>
-      <c r="D2" s="4" t="n">
+      <c r="C2" s="4">
+        <v>72.822693999999998</v>
+      </c>
+      <c r="D2" s="4">
         <v>50</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>422</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>80</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>120</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="n">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
         <v>720</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2">
         <v>1020</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2">
         <v>120</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -891,48 +1094,48 @@
       <c r="Q2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>18.922249</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>72.833697</v>
-      </c>
-      <c r="D3" s="1" t="n">
+    <row r="3" spans="1:18">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18.922249000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>72.833697000000001</v>
+      </c>
+      <c r="D3" s="1">
         <v>45</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>288</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>120</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>120</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="n">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
         <v>720</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3">
         <v>900</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3">
         <v>60</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -948,8 +1151,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:18">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -958,40 +1161,40 @@
       <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>25</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>200</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>300</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="n">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
         <v>30</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4">
         <v>930</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4">
         <v>90</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" t="s">
         <v>30</v>
       </c>
       <c r="P4" s="2" t="s">
@@ -999,8 +1202,8 @@
       </c>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:18">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1009,40 +1212,40 @@
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>35</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>400</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="n">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
         <v>120</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5">
         <v>660</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5">
         <v>120</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="O5" t="s">
         <v>35</v>
       </c>
       <c r="P5" s="2" t="s">
@@ -1050,8 +1253,8 @@
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:18">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1060,34 +1263,34 @@
       <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>1800</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="n">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
         <v>300</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6">
         <v>360</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6">
         <v>420</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -1099,15 +1302,15 @@
       <c r="P6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" t="s">
         <v>42</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="R6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:18">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1116,34 +1319,34 @@
       <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>40</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>331</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>100</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>60</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="n">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
         <v>810</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7">
         <v>1020</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7">
         <v>120</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -1159,8 +1362,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:18">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1169,40 +1372,40 @@
       <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>15</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>590</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="n">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <v>720</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8">
         <v>960</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8">
         <v>180</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="0" t="s">
+      <c r="O8" t="s">
         <v>52</v>
       </c>
       <c r="P8" s="2" t="s">
@@ -1212,8 +1415,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:18">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1222,54 +1425,54 @@
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>35</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9">
         <v>216</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>50</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>70</v>
       </c>
-      <c r="I9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="n">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
         <v>870</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9">
         <v>1080</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9">
         <v>60</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="O9" t="s">
         <v>58</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" t="s">
         <v>60</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:18">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1278,40 +1481,40 @@
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>10</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10">
         <v>700</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10">
         <v>80</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="n">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
         <v>240</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10">
         <v>420</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10">
         <v>240</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="O10" t="s">
         <v>65</v>
       </c>
       <c r="P10" s="2" t="s">
@@ -1321,8 +1524,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:18">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1331,40 +1534,40 @@
       <c r="C11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>15</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11">
         <v>100</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11">
         <v>250</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1" t="n">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
         <v>180</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11">
         <v>645</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11">
         <v>90</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="O11" t="s">
         <v>71</v>
       </c>
       <c r="P11" s="2" t="s">
@@ -1372,8 +1575,8 @@
       </c>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:18">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1382,40 +1585,40 @@
       <c r="C12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>20</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>90</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1" t="n">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
         <v>360</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12">
         <v>810</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12">
         <v>30</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O12" s="0" t="s">
+      <c r="O12" t="s">
         <v>76</v>
       </c>
       <c r="P12" s="2" t="s">
@@ -1424,12 +1627,12 @@
       <c r="Q12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="R12" s="0" t="s">
+      <c r="R12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:18">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1438,40 +1641,40 @@
       <c r="C13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>10</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13">
         <v>200</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>200</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="n">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
         <v>240</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13">
         <v>510</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13">
         <v>240</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O13" s="0" t="s">
+      <c r="O13" t="s">
         <v>83</v>
       </c>
       <c r="P13" s="2" t="s">
@@ -1480,51 +1683,51 @@
       <c r="Q13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R13" s="0" t="s">
+      <c r="R13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:18" ht="17.850000000000001" customHeight="1">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>19.0505835</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>72.8192191</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="B14">
+        <v>19.050583499999998</v>
+      </c>
+      <c r="C14">
+        <v>72.819219099999998</v>
+      </c>
+      <c r="D14">
         <v>45</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14">
         <v>350</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="0" t="n">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>100</v>
       </c>
-      <c r="I14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="0" t="n">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>720</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14">
         <v>900</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14">
         <v>120</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" t="s">
         <v>87</v>
       </c>
       <c r="O14" s="5" t="s">
@@ -1536,12 +1739,12 @@
       <c r="Q14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="R14" s="0" t="s">
+      <c r="R14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:18">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1550,40 +1753,40 @@
       <c r="C15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>10</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15">
         <v>250</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15">
         <v>500</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="n">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
         <v>180</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15">
         <v>810</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15">
         <v>240</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O15" s="0" t="s">
+      <c r="O15" t="s">
         <v>94</v>
       </c>
       <c r="P15" s="2" t="s">
@@ -1593,8 +1796,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:18">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1603,40 +1806,40 @@
       <c r="C16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="0" t="n">
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>50</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="0" t="n">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>400</v>
       </c>
-      <c r="J16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="n">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
         <v>690</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16">
         <v>840</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16">
         <v>120</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O16" s="0" t="s">
+      <c r="O16" t="s">
         <v>100</v>
       </c>
       <c r="P16" s="2" t="s">
@@ -1646,58 +1849,58 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:18" ht="17.850000000000001" customHeight="1">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>18.9272722</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>72.8318454</v>
-      </c>
-      <c r="D17" s="0" t="n">
+      <c r="B17">
+        <v>18.927272200000001</v>
+      </c>
+      <c r="C17">
+        <v>72.831845400000006</v>
+      </c>
+      <c r="D17">
         <v>40</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17">
         <v>350</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17">
         <v>50</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="0" t="n">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>360</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17">
         <v>660</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17">
         <v>120</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="O17" s="0" t="s">
+      <c r="O17" t="s">
         <v>103</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:18">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1706,34 +1909,34 @@
       <c r="C18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>30</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18">
         <v>300</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="0" t="n">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
         <v>50</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="n">
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
         <v>720</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18">
         <v>780</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18">
         <v>75</v>
       </c>
       <c r="N18" s="1" t="s">
@@ -1749,8 +1952,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:18">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1759,40 +1962,40 @@
       <c r="C19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" s="0" t="n">
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <v>150</v>
       </c>
-      <c r="J19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="n">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
         <v>690</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19">
         <v>840</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19">
         <v>90</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="O19" s="0" t="s">
+      <c r="O19" t="s">
         <v>114</v>
       </c>
       <c r="P19" s="2" t="s">
@@ -1802,8 +2005,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:18">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1812,40 +2015,40 @@
       <c r="C20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="0" t="n">
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>400</v>
       </c>
-      <c r="J20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1" t="n">
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
         <v>690</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20">
         <v>840</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20">
         <v>120</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="O20" s="0" t="s">
+      <c r="O20" t="s">
         <v>114</v>
       </c>
       <c r="P20" s="2" t="s">
@@ -1855,159 +2058,159 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:18">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21">
         <v>19.1393792</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <v>72.8434279</v>
-      </c>
-      <c r="D21" s="0" t="n">
+      <c r="C21">
+        <v>72.843427899999995</v>
+      </c>
+      <c r="D21">
         <v>15</v>
       </c>
-      <c r="E21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="0" t="n">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
         <v>350</v>
       </c>
-      <c r="I21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="0" t="n">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
         <v>810</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21">
         <v>960</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21">
         <v>180</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="0" t="s">
+      <c r="O21" t="s">
         <v>123</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="P21" t="s">
         <v>124</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="Q21" t="s">
         <v>125</v>
       </c>
-      <c r="R21" s="0" t="s">
+      <c r="R21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:18" ht="20.85" customHeight="1">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>19.0007441</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>72.8273683</v>
-      </c>
-      <c r="D22" s="0" t="n">
+      <c r="B22">
+        <v>19.000744099999999</v>
+      </c>
+      <c r="C22">
+        <v>72.827368300000003</v>
+      </c>
+      <c r="D22">
         <v>15</v>
       </c>
-      <c r="E22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="0" t="n">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>400</v>
       </c>
-      <c r="I22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="0" t="n">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
         <v>810</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22">
         <v>960</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="M22">
         <v>180</v>
       </c>
-      <c r="N22" s="0" t="s">
+      <c r="N22" t="s">
         <v>127</v>
       </c>
-      <c r="O22" s="0" t="s">
+      <c r="O22" t="s">
         <v>123</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="Q22" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:18">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="n">
-        <v>18.9900943</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>72.812512</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="B23" s="1">
+        <v>18.990094299999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>72.812511999999998</v>
+      </c>
+      <c r="D23" s="1">
         <v>15</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23">
         <v>295</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="0" t="n">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
         <v>100</v>
       </c>
-      <c r="H23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1" t="n">
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
         <v>570</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="L23">
         <v>600</v>
       </c>
-      <c r="M23" s="0" t="n">
+      <c r="M23">
         <v>120</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O23" s="0" t="s">
+      <c r="O23" t="s">
         <v>131</v>
       </c>
       <c r="P23" s="2" t="s">
@@ -2017,197 +2220,197 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="n">
-        <v>18.990556</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>72.8159062</v>
-      </c>
-      <c r="D24" s="1" t="n">
+      <c r="B24" s="1">
+        <v>18.990556000000002</v>
+      </c>
+      <c r="C24" s="1">
+        <v>72.815906200000001</v>
+      </c>
+      <c r="D24" s="1">
         <v>30</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24">
         <v>612</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
         <v>150</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1" t="n">
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
         <v>300</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24">
         <v>480</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="M24">
         <v>180</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="O24" s="0" t="s">
+      <c r="O24" t="s">
         <v>135</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:18">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="1">
         <v>19.0465166</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="1">
         <v>72.8202383</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="1">
         <v>10</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25">
         <v>100</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>200</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1" t="n">
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
         <v>300</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25">
         <v>600</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25">
         <v>45</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="O25" s="0" t="s">
+      <c r="O25" t="s">
         <v>138</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:18">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="n">
-        <v>18.9950587</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>72.8223205</v>
-      </c>
-      <c r="D26" s="1" t="n">
+      <c r="B26" s="1">
+        <v>18.995058700000001</v>
+      </c>
+      <c r="C26" s="1">
+        <v>72.822320500000004</v>
+      </c>
+      <c r="D26" s="1">
         <v>15</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26">
         <v>200</v>
       </c>
-      <c r="F26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="0" t="n">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
         <v>100</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26">
         <v>200</v>
       </c>
-      <c r="J26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1" t="n">
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
         <v>420</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="L26">
         <v>900</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26">
         <v>120</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" t="s">
         <v>141</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="Q26" s="0" t="s">
+      <c r="Q26" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:18">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>19.1760434</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>72.7904668</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="0" t="n">
+      <c r="B27" s="1">
+        <v>19.176043400000001</v>
+      </c>
+      <c r="C27" s="1">
+        <v>72.790466800000004</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>280</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="0" t="n">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
         <v>100</v>
       </c>
-      <c r="H27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="n">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
         <v>60</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="L27">
         <v>360</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="M27">
         <v>120</v>
       </c>
       <c r="N27" s="1" t="s">
@@ -2220,383 +2423,378 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:18">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="n">
-        <v>18.9577291</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>72.8077108</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" s="0" t="n">
+      <c r="B28" s="1">
+        <v>18.957729100000002</v>
+      </c>
+      <c r="C28" s="1">
+        <v>72.807710799999995</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28">
         <v>130</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28">
         <v>100</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="0" t="n">
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
         <v>360</v>
       </c>
-      <c r="M28" s="0" t="n">
+      <c r="M28">
         <v>60</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O28" s="0" t="s">
+      <c r="O28" t="s">
         <v>108</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:18">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>19.113082</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>72.8240954</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="0" t="n">
+      <c r="B29">
+        <v>19.113081999999999</v>
+      </c>
+      <c r="C29">
+        <v>72.824095400000004</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
         <v>100</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29">
         <v>300</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="0" t="n">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
         <v>360</v>
       </c>
-      <c r="M29" s="0" t="n">
+      <c r="M29">
         <v>120</v>
       </c>
-      <c r="N29" s="0" t="s">
+      <c r="N29" t="s">
         <v>148</v>
       </c>
-      <c r="O29" s="0" t="s">
+      <c r="O29" t="s">
         <v>108</v>
       </c>
       <c r="P29" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:18">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>19.1225268</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>72.9117135</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="0" t="n">
+      <c r="B30">
+        <v>19.122526799999999</v>
+      </c>
+      <c r="C30">
+        <v>72.911713500000005</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
         <v>100</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="0" t="n">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
         <v>450</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" s="0" t="n">
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
         <v>660</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="L30">
         <v>840</v>
       </c>
-      <c r="M30" s="0" t="n">
+      <c r="M30">
         <v>180</v>
       </c>
-      <c r="N30" s="0" t="s">
+      <c r="N30" t="s">
         <v>150</v>
       </c>
-      <c r="O30" s="0" t="s">
+      <c r="O30" t="s">
         <v>151</v>
       </c>
-      <c r="P30" s="0" t="s">
+      <c r="P30" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:18">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31">
         <v>19.0046195</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31">
         <v>72.8238834</v>
       </c>
-      <c r="D31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="0" t="n">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
         <v>550</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31">
         <v>300</v>
       </c>
-      <c r="I31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" s="0" t="n">
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
         <v>810</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L31">
         <v>960</v>
       </c>
-      <c r="M31" s="0" t="n">
+      <c r="M31">
         <v>210</v>
       </c>
-      <c r="N31" s="0" t="s">
+      <c r="N31" t="s">
         <v>153</v>
       </c>
-      <c r="O31" s="0" t="s">
+      <c r="O31" t="s">
         <v>154</v>
       </c>
-      <c r="P31" s="0" t="s">
+      <c r="P31" t="s">
         <v>155</v>
       </c>
-      <c r="Q31" s="0" t="s">
+      <c r="Q31" t="s">
         <v>156</v>
       </c>
-      <c r="R31" s="0" t="s">
+      <c r="R31" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:18">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>19.0066993</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>72.827239</v>
-      </c>
-      <c r="D32" s="0" t="n">
+      <c r="B32">
+        <v>19.006699300000001</v>
+      </c>
+      <c r="C32">
+        <v>72.827239000000006</v>
+      </c>
+      <c r="D32">
         <v>15</v>
       </c>
-      <c r="E32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="0" t="n">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
         <v>450</v>
       </c>
-      <c r="I32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="0" t="n">
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
         <v>810</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="L32">
         <v>990</v>
       </c>
-      <c r="M32" s="0" t="n">
+      <c r="M32">
         <v>180</v>
       </c>
-      <c r="N32" s="0" t="s">
+      <c r="N32" t="s">
         <v>158</v>
       </c>
-      <c r="O32" s="0" t="s">
+      <c r="O32" t="s">
         <v>159</v>
       </c>
-      <c r="P32" s="0" t="s">
+      <c r="P32" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:18">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33">
         <v>19.0997156</v>
       </c>
-      <c r="C33" s="0" t="n">
-        <v>72.9142367</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" s="0" t="n">
+      <c r="C33">
+        <v>72.914236700000004</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
         <v>300</v>
       </c>
-      <c r="I33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="0" t="n">
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
         <v>810</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="L33">
         <v>990</v>
       </c>
-      <c r="M33" s="0" t="n">
+      <c r="M33">
         <v>150</v>
       </c>
-      <c r="N33" s="0" t="s">
+      <c r="N33" t="s">
         <v>161</v>
       </c>
-      <c r="O33" s="0" t="s">
+      <c r="O33" t="s">
         <v>162</v>
       </c>
-      <c r="P33" s="0" t="s">
+      <c r="P33" t="s">
         <v>163</v>
       </c>
-      <c r="Q33" s="0" t="s">
+      <c r="Q33" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:18" ht="14.1" customHeight="1">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>18.9215861</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>72.8301393</v>
-      </c>
-      <c r="D34" s="0" t="n">
+      <c r="B34">
+        <v>18.921586099999999</v>
+      </c>
+      <c r="C34">
+        <v>72.830139299999999</v>
+      </c>
+      <c r="D34">
         <v>10</v>
       </c>
-      <c r="E34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" s="0" t="n">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
         <v>400</v>
       </c>
-      <c r="I34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="0" t="n">
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
         <v>810</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L34">
         <v>960</v>
       </c>
-      <c r="M34" s="0" t="n">
+      <c r="M34">
         <v>150</v>
       </c>
-      <c r="N34" s="0" t="s">
+      <c r="N34" t="s">
         <v>165</v>
       </c>
-      <c r="O34" s="0" t="s">
+      <c r="O34" t="s">
         <v>166</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="Q34" s="0" t="s">
+      <c r="Q34" t="s">
         <v>168</v>
       </c>
-      <c r="R34" s="0" t="s">
+      <c r="R34" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" spans="1:18" ht="20.85" customHeight="1"/>
+    <row r="37" spans="1:18" ht="17.850000000000001" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R6" r:id="rId1" display="P.P.S : Check www.esselworld.in for offers"/>
+    <hyperlink ref="R6" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>